<commit_message>
added features and cleared features
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_codes_location.xlsx
+++ b/whonet/static/whonet_xl/whonet_codes_location.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="772" firstSheet="13" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="772"/>
   </bookViews>
   <sheets>
     <sheet name="bgh" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">feu!$A$1:$E$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">vsm!$A$1:$E$97</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4034,8 +4034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4248,7 +4248,7 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -30077,8 +30077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30355,7 +30355,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>